<commit_message>
Report Matching - fix row heights
</commit_message>
<xml_diff>
--- a/public/downloads/Template Files/Aged Payables Report Result.xlsx
+++ b/public/downloads/Template Files/Aged Payables Report Result.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RMG\Documents\Task\1-26~Excel Link\Template Files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RMG\Documents\vs1_cloud_project\public\downloads\Template Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3609B4A9-8A16-4987-8AFE-3B7D49064AC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8E36E0D-7EE1-4A1C-B39C-EAAA1832FEB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29010" windowHeight="13560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1288,7 +1288,7 @@
   <numFmts count="1">
     <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1307,6 +1307,14 @@
       <color theme="1"/>
       <name val="Segoe UI"/>
       <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -1329,7 +1337,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1339,6 +1347,9 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -2103,7 +2114,7 @@
   <dimension ref="A1:I26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2120,31 +2131,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="5" t="s">
         <v>380</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="5" t="s">
         <v>381</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="5" t="s">
         <v>382</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="5" t="s">
         <v>383</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="5" t="s">
         <v>384</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="5" t="s">
         <v>385</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="5" t="s">
         <v>386</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="5" t="s">
         <v>387</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I1" s="5" t="s">
         <v>388</v>
       </c>
     </row>
@@ -2747,6 +2758,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>